<commit_message>
config: pre-commit hooks improved
</commit_message>
<xml_diff>
--- a/static/xlsx/Etkinlik Takvimi.xlsx
+++ b/static/xlsx/Etkinlik Takvimi.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="0"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>İsim</t>
   </si>
@@ -247,28 +241,47 @@
     <t>22.05.2023</t>
   </si>
   <si>
+    <t>Turkcell Ankara Üniversiteler Buluşması</t>
+  </si>
+  <si>
+    <t>13.06.2023</t>
+  </si>
+  <si>
+    <t>STM ile Siber Güvenlik Söyleşisi</t>
+  </si>
+  <si>
+    <t>20.06.2023</t>
+  </si>
+  <si>
     <t>Siber Güvenlik Kulübü</t>
   </si>
   <si>
-    <t>STM ile Siber Güvenlik Söyleşisi</t>
-  </si>
-  <si>
     <t>HAVELSAN ile Yazılım - İnovasyon Webinarı</t>
-  </si>
-  <si>
-    <t>20.06.2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -276,27 +289,355 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -304,126 +645,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -681,28 +1204,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A21">
-      <selection pane="topLeft" activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.004285714285713" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="31.571428571428573" customWidth="1"/>
-    <col min="2" max="2" width="10.714285714285714" customWidth="1"/>
-    <col min="3" max="3" width="12.857142857142858" customWidth="1"/>
+    <col min="1" max="1" width="31.5740740740741" customWidth="1"/>
+    <col min="2" max="2" width="10.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="12.8611111111111" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="18.142857142857142" customWidth="1"/>
+    <col min="6" max="6" width="18.1388888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,7 +1243,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -728,16 +1251,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D2" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -745,16 +1268,16 @@
         <v>9</v>
       </c>
       <c r="C3" s="2">
-        <v>0.58333333333333304</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="D3" s="2">
-        <v>0.70833333333333304</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -771,7 +1294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -779,16 +1302,16 @@
         <v>14</v>
       </c>
       <c r="C5" s="2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -799,13 +1322,13 @@
         <v>0.75</v>
       </c>
       <c r="D6" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -813,7 +1336,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>0.41666666666666702</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="D7" s="2">
         <v>0.75</v>
@@ -822,7 +1345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -833,13 +1356,13 @@
         <v>0.625</v>
       </c>
       <c r="D8" s="2">
-        <v>0.70833333333333304</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -847,7 +1370,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="2">
-        <v>0.60416666666666696</v>
+        <v>0.604166666666667</v>
       </c>
       <c r="D9" s="2">
         <v>0.6875</v>
@@ -856,7 +1379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -864,16 +1387,16 @@
         <v>25</v>
       </c>
       <c r="C10" s="2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -881,16 +1404,16 @@
         <v>27</v>
       </c>
       <c r="C11" s="2">
-        <v>0.60416666666666696</v>
+        <v>0.604166666666667</v>
       </c>
       <c r="D11" s="2">
-        <v>0.70833333333333304</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -898,16 +1421,16 @@
         <v>29</v>
       </c>
       <c r="C12" s="2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -915,7 +1438,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="2">
-        <v>0.41666666666666702</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="D13" s="2">
         <v>0.75</v>
@@ -924,7 +1447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -932,16 +1455,16 @@
         <v>33</v>
       </c>
       <c r="C14" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D14" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -949,7 +1472,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="2">
-        <v>0.41666666666666702</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="D15" s="2">
         <v>0.625</v>
@@ -958,7 +1481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -966,16 +1489,16 @@
         <v>37</v>
       </c>
       <c r="C16" s="2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -986,13 +1509,13 @@
         <v>0.75</v>
       </c>
       <c r="D17" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1000,16 +1523,16 @@
         <v>41</v>
       </c>
       <c r="C18" s="2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1017,7 +1540,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="2">
-        <v>0.66666666666666696</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="D19" s="2">
         <v>0.75</v>
@@ -1026,7 +1549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1034,16 +1557,16 @@
         <v>45</v>
       </c>
       <c r="C20" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D20" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1051,7 +1574,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="2">
-        <v>0.66666666666666696</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="D21" s="2">
         <v>0.75</v>
@@ -1060,7 +1583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1068,16 +1591,16 @@
         <v>49</v>
       </c>
       <c r="C22" s="2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="2">
-        <v>0.54166666666666696</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1088,13 +1611,13 @@
         <v>0.625</v>
       </c>
       <c r="D23" s="2">
-        <v>0.70833333333333304</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1102,7 +1625,7 @@
         <v>53</v>
       </c>
       <c r="C24" s="2">
-        <v>0.66666666666666696</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="D24" s="2">
         <v>0.75</v>
@@ -1111,7 +1634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1119,16 +1642,16 @@
         <v>55</v>
       </c>
       <c r="C25" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D25" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1139,13 +1662,13 @@
         <v>0.875</v>
       </c>
       <c r="D26" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1162,7 +1685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1170,16 +1693,16 @@
         <v>61</v>
       </c>
       <c r="C28" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D28" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1187,7 +1710,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="2">
-        <v>0.72916666666666696</v>
+        <v>0.729166666666667</v>
       </c>
       <c r="D29" s="2">
         <v>0.75</v>
@@ -1196,7 +1719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1213,7 +1736,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1221,7 +1744,7 @@
         <v>68</v>
       </c>
       <c r="C31" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D31" s="2">
         <v>0.875</v>
@@ -1230,7 +1753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1241,13 +1764,13 @@
         <v>0.8125</v>
       </c>
       <c r="D32" s="2">
-        <v>0.85416666666666696</v>
+        <v>0.854166666666667</v>
       </c>
       <c r="E32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1255,16 +1778,16 @@
         <v>72</v>
       </c>
       <c r="C33" s="2">
-        <v>0.77083333333333304</v>
+        <v>0.770833333333333</v>
       </c>
       <c r="D33" s="2">
-        <v>0.79166666666666696</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="E33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -1272,33 +1795,33 @@
         <v>74</v>
       </c>
       <c r="C34" s="2">
-        <v>0.79166666666666696</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="D34" s="2">
-        <v>0.95833333333333304</v>
+        <v>0.958333333333333</v>
       </c>
       <c r="E34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C35" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="D35" s="2">
-        <v>0.75</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -1306,16 +1829,34 @@
         <v>78</v>
       </c>
       <c r="C36" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D36" s="4">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D37" s="4">
         <v>0.875</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Etkinlik takvimi Hata Düzeltme
Excel tablo formatı düzeltildi.
</commit_message>
<xml_diff>
--- a/static/xlsx/Etkinlik Takvimi.xlsx
+++ b/static/xlsx/Etkinlik Takvimi.xlsx
@@ -37,9 +37,6 @@
     <t xml:space="preserve">Düzenleyen</t>
   </si>
   <si>
-    <t xml:space="preserve">Katılımcı Sayısı</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kuruluş Toplantısı</t>
   </si>
   <si>
@@ -283,13 +280,16 @@
     <t xml:space="preserve">Buğra Ayan ile Finansal Teknolojiler ve Geleceği</t>
   </si>
   <si>
+    <t xml:space="preserve">03.09.2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">Melih Turan ile Finansın Dijital Dönüşümü</t>
   </si>
   <si>
     <t xml:space="preserve">09.08.2023</t>
   </si>
   <si>
-    <t xml:space="preserve">05.09.2023/06.09.2023</t>
+    <t xml:space="preserve">05.09.2023</t>
   </si>
   <si>
     <t xml:space="preserve">Archis Academy Eğitim</t>
@@ -419,10 +419,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -434,7 +434,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,16 +450,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>0.833333333333333</v>
@@ -468,18 +465,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0.583333333333333</v>
@@ -488,18 +482,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0.625</v>
@@ -508,18 +499,15 @@
         <v>0.75</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0.5</v>
@@ -528,18 +516,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0.75</v>
@@ -548,18 +533,15 @@
         <v>0.833333333333333</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>0.416666666666667</v>
@@ -568,18 +550,15 @@
         <v>0.75</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0.625</v>
@@ -588,18 +567,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0.604166666666667</v>
@@ -608,18 +584,15 @@
         <v>0.6875</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.5</v>
@@ -628,18 +601,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>0.604166666666667</v>
@@ -648,18 +618,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0.5</v>
@@ -668,18 +635,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="0" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0.416666666666667</v>
@@ -688,18 +652,15 @@
         <v>0.75</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>0.833333333333333</v>
@@ -708,18 +669,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0.416666666666667</v>
@@ -728,18 +686,15 @@
         <v>0.625</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0.5</v>
@@ -748,18 +703,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0.75</v>
@@ -768,18 +720,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0.5</v>
@@ -788,18 +737,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>0.666666666666667</v>
@@ -808,18 +754,15 @@
         <v>0.75</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>0.833333333333333</v>
@@ -828,18 +771,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0.666666666666667</v>
@@ -848,18 +788,15 @@
         <v>0.75</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>50</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0.5</v>
@@ -868,18 +805,15 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>0.625</v>
@@ -888,18 +822,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0.666666666666667</v>
@@ -908,18 +839,15 @@
         <v>0.75</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>0.833333333333333</v>
@@ -928,18 +856,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>0.875</v>
@@ -948,18 +873,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0.6875</v>
@@ -968,18 +890,15 @@
         <v>0.8125</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>0.833333333333333</v>
@@ -988,18 +907,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>0.729166666666667</v>
@@ -1008,18 +924,15 @@
         <v>0.75</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>0.875</v>
@@ -1028,18 +941,15 @@
         <v>0.9375</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="B31" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>0.833333333333333</v>
@@ -1048,18 +958,15 @@
         <v>0.875</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>0.8125</v>
@@ -1068,18 +975,15 @@
         <v>0.854166666666667</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>0.770833333333333</v>
@@ -1088,18 +992,15 @@
         <v>0.791666666666667</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>0.791666666666667</v>
@@ -1108,18 +1009,15 @@
         <v>0.958333333333333</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>0.583333333333333</v>
@@ -1128,18 +1026,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0.666666666666667</v>
@@ -1148,18 +1043,15 @@
         <v>0.75</v>
       </c>
       <c r="E36" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F36" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="B37" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>0.833333333333333</v>
@@ -1168,18 +1060,15 @@
         <v>0.875</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>83</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0.520833333333333</v>
@@ -1188,18 +1077,15 @@
         <v>0.583333333333333</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0.833333333333333</v>
@@ -1208,14 +1094,14 @@
         <v>0.895833333333333</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>86</v>
       </c>
       <c r="C40" s="2" t="n">
@@ -1225,13 +1111,10 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>87</v>
       </c>
@@ -1245,15 +1128,12 @@
         <v>0.875</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>89</v>
@@ -1265,10 +1145,7 @@
         <v>0.75</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,7 +1162,7 @@
         <v>0.875</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>